<commit_message>
Improve design and increased the number of images upload
</commit_message>
<xml_diff>
--- a/templates/email_template.xlsx
+++ b/templates/email_template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sgvggroup-my.sharepoint.com/personal/neeraj_balodi_sgvgroup_in/Documents/Desktop/Rajesh Sir/Daily Vigilance Report/templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sgvggroup-my.sharepoint.com/personal/neeraj_balodi_sgvgroup_in/Documents/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="13_ncr:1_{BA34A785-6692-40F1-91E6-E7AFCFFF45F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3D3BD14C-1A3C-46CD-9537-4B51887DD49F}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{E27168ED-051A-47AD-A684-8E4E219F9100}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{998110AF-D3AF-4518-99AE-9565B898E903}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="70">
   <si>
     <t>Date</t>
   </si>
@@ -91,18 +91,15 @@
     <t>Site Safety</t>
   </si>
   <si>
-    <t>Documentation &amp; Equipment</t>
-  </si>
-  <si>
     <t>Overall Rating</t>
   </si>
   <si>
-    <t>Suggestion</t>
-  </si>
-  <si>
     <t>Inspected By</t>
   </si>
   <si>
+    <t>Night</t>
+  </si>
+  <si>
     <t>Impressive</t>
   </si>
   <si>
@@ -112,13 +109,161 @@
     <t>Satisfactory</t>
   </si>
   <si>
-    <t>Image 1</t>
-  </si>
-  <si>
-    <t>Image 2</t>
-  </si>
-  <si>
-    <t>Image 3</t>
+    <t>rajesh.dahiya@sgvgroup.in</t>
+  </si>
+  <si>
+    <t>vikas.datika@sgvgroup.in</t>
+  </si>
+  <si>
+    <t>Mr. Sumit</t>
+  </si>
+  <si>
+    <t>Mr. Parmeet</t>
+  </si>
+  <si>
+    <t>Downtown &amp; Downtown Project</t>
+  </si>
+  <si>
+    <t>Surface Parking 03</t>
+  </si>
+  <si>
+    <t>Infinity Tower Road Team</t>
+  </si>
+  <si>
+    <t>CGS Hospital</t>
+  </si>
+  <si>
+    <t>Phase 3 QRT</t>
+  </si>
+  <si>
+    <t>DLF Land Phase 3</t>
+  </si>
+  <si>
+    <t>Surface Parking 06</t>
+  </si>
+  <si>
+    <t>SR.NO</t>
+  </si>
+  <si>
+    <t>Nth 90</t>
+  </si>
+  <si>
+    <t>Mapsko Casa Bella</t>
+  </si>
+  <si>
+    <t>Bestech Grand Spa</t>
+  </si>
+  <si>
+    <t>Guards were well-groomed and in full uniform — a commendable standard of appearance.</t>
+  </si>
+  <si>
+    <t>Guards displayed high levels of alertness and responded promptly during checks.</t>
+  </si>
+  <si>
+    <t>All registers were properly updated and well-organized — reflects good documentation discipline.</t>
+  </si>
+  <si>
+    <t>Guards were aware of emergency exits and briefed on evacuation protocols.</t>
+  </si>
+  <si>
+    <t>Team demonstrated excellent coordination and professionalism throughout the inspection.</t>
+  </si>
+  <si>
+    <t>All security equipment was fully functional and readily available.</t>
+  </si>
+  <si>
+    <t>Post area was clean and well-maintained; excellent housekeeping by the deployed team.</t>
+  </si>
+  <si>
+    <t>Torch lights and walkie-talkies were charged and tested — readiness appreciated.</t>
+  </si>
+  <si>
+    <t>Effective patrolling observed throughout the shift, maintaining strong site coverage.</t>
+  </si>
+  <si>
+    <t>Tarc Maceo</t>
+  </si>
+  <si>
+    <t>neeraj.balodi@sgvgroup.in</t>
+  </si>
+  <si>
+    <t>vikas.datika@sgvgroup.in; neeraj.balodi@sgvgroup.in</t>
+  </si>
+  <si>
+    <t>Contact Person</t>
+  </si>
+  <si>
+    <t>Attendance Register</t>
+  </si>
+  <si>
+    <t>Handling/Taking Over Register</t>
+  </si>
+  <si>
+    <t>Material In / Out Register</t>
+  </si>
+  <si>
+    <t>Shortage</t>
+  </si>
+  <si>
+    <t>Mobiles (Shift Cell)</t>
+  </si>
+  <si>
+    <t>HHMD</t>
+  </si>
+  <si>
+    <t>Torch</t>
+  </si>
+  <si>
+    <t>Batten</t>
+  </si>
+  <si>
+    <t>Observation</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>nil</t>
+  </si>
+  <si>
+    <t>02- S/G</t>
+  </si>
+  <si>
+    <t>02-S/G</t>
+  </si>
+  <si>
+    <t>01-SO
+02-S/G</t>
+  </si>
+  <si>
+    <t>02-Working</t>
+  </si>
+  <si>
+    <t>01-Not working</t>
+  </si>
+  <si>
+    <t>DLF</t>
+  </si>
+  <si>
+    <t>Tarc</t>
+  </si>
+  <si>
+    <t>Mapsko Group</t>
+  </si>
+  <si>
+    <t>Bestech</t>
+  </si>
+  <si>
+    <t>Mr. Rajesh</t>
+  </si>
+  <si>
+    <t>Mr. Neeraj</t>
+  </si>
+  <si>
+    <t>Other Security Equipments</t>
+  </si>
+  <si>
+    <t>Working - 02; Not Working - 01</t>
   </si>
 </sst>
 </file>
@@ -638,24 +783,43 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="18" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="42" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="42" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -1013,212 +1177,1044 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA5"/>
+  <dimension ref="A1:AH12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="A2" sqref="A2:Z12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.26953125" customWidth="1"/>
-    <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="8.6328125" customWidth="1"/>
-    <col min="4" max="4" width="7.453125" customWidth="1"/>
-    <col min="5" max="5" width="13.26953125" customWidth="1"/>
-    <col min="6" max="6" width="16.6328125" customWidth="1"/>
-    <col min="7" max="7" width="18.6328125" customWidth="1"/>
-    <col min="8" max="8" width="14.1796875" customWidth="1"/>
-    <col min="9" max="9" width="13" customWidth="1"/>
-    <col min="10" max="10" width="12.1796875" customWidth="1"/>
-    <col min="11" max="11" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.453125" customWidth="1"/>
-    <col min="14" max="14" width="12.36328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="29.1796875" customWidth="1"/>
-    <col min="16" max="16" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.1796875" customWidth="1"/>
-    <col min="18" max="18" width="12.453125" customWidth="1"/>
-    <col min="19" max="19" width="11.36328125" customWidth="1"/>
-    <col min="26" max="26" width="11.54296875" customWidth="1"/>
+    <col min="1" max="1" width="6.08984375" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.08984375" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.90625" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.7265625" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23" style="9" customWidth="1"/>
+    <col min="10" max="10" width="28.36328125" style="9" customWidth="1"/>
+    <col min="11" max="11" width="17.6328125" style="9" customWidth="1"/>
+    <col min="12" max="12" width="14.453125" style="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.81640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.1796875" style="9" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11" style="5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="19" max="21" width="13.6328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.36328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="34.26953125" style="11" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.36328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="11.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="6" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="I1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="J1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="K1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="P1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="Q1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="R1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="S1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="X1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="Y1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="AG1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AH1" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6">
+        <v>45769</v>
+      </c>
+      <c r="C2" s="7">
+        <v>0.40277777777777779</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="5" t="s">
+      <c r="E2" s="4">
+        <v>1</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="N2" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="S2" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="T2" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="U2" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="V2" s="4">
+        <v>5</v>
+      </c>
+      <c r="W2" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="X2" s="4" t="str" cm="1">
+        <f t="array" ref="X2">INDEX({"Satisfactory","Impressive","Outstanding"},MAX(1,ROUND(AVERAGE(MATCH(O2:R2,{"Satisfactory","Impressive","Outstanding"},0)),0)))</f>
+        <v>Impressive</v>
+      </c>
+      <c r="Y2" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z2" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6">
+        <v>45770</v>
+      </c>
+      <c r="C3" s="7">
+        <v>4.0972222222222222E-2</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="4">
+        <v>1</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="M3" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="R3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="S3" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="T3" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="U3" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="V3" s="4">
+        <v>3</v>
+      </c>
+      <c r="W3" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="X3" s="4" t="str" cm="1">
+        <f t="array" ref="X3">INDEX({"Satisfactory","Impressive","Outstanding"},MAX(1,ROUND(AVERAGE(MATCH(O3:R3,{"Satisfactory","Impressive","Outstanding"},0)),0)))</f>
+        <v>Impressive</v>
+      </c>
+      <c r="Y3" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="Z3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="AG3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AH3" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6">
+        <v>45770</v>
+      </c>
+      <c r="C4" s="7">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="4">
+        <v>1</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="I4" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="J4" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="M4" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="N4" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="P4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="R4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="S4" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="T4" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="U4" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="V4" s="4">
+        <v>5</v>
+      </c>
+      <c r="W4" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="X4" s="4" t="str" cm="1">
+        <f t="array" ref="X4">INDEX({"Satisfactory","Impressive","Outstanding"},MAX(1,ROUND(AVERAGE(MATCH(O4:R4,{"Satisfactory","Impressive","Outstanding"},0)),0)))</f>
+        <v>Impressive</v>
+      </c>
+      <c r="Y4" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="AG4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="AH4" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6">
+        <v>45770</v>
+      </c>
+      <c r="C5" s="7">
+        <v>5.6250000000000001E-2</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="4">
+        <v>2</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="L5" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="M5" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="N5" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="P5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="R5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="S5" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="T5" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="U5" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="V5" s="4">
+        <v>4</v>
+      </c>
+      <c r="W5" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="X5" s="4" t="str" cm="1">
+        <f t="array" ref="X5">INDEX({"Satisfactory","Impressive","Outstanding"},MAX(1,ROUND(AVERAGE(MATCH(O5:R5,{"Satisfactory","Impressive","Outstanding"},0)),0)))</f>
+        <v>Impressive</v>
+      </c>
+      <c r="Y5" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z5" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:34" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6">
+        <v>45770</v>
+      </c>
+      <c r="C6" s="7">
+        <v>6.7361111111111108E-2</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="4">
+        <v>2</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="L6" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="M6" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="N6" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="O6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="P6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="R6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="S6" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="T6" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="U6" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="V6" s="4">
+        <v>3</v>
+      </c>
+      <c r="W6" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="X6" s="4" t="str" cm="1">
+        <f t="array" ref="X6">INDEX({"Satisfactory","Impressive","Outstanding"},MAX(1,ROUND(AVERAGE(MATCH(O6:R6,{"Satisfactory","Impressive","Outstanding"},0)),0)))</f>
+        <v>Impressive</v>
+      </c>
+      <c r="Y6" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z6" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6">
+        <v>45770</v>
+      </c>
+      <c r="C7" s="7">
+        <v>0.16527777777777777</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="4">
+        <v>2</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="L7" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="M7" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="N7" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="O7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="P7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="R7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="S7" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="T7" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="U7" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="V7" s="4">
+        <v>4</v>
+      </c>
+      <c r="W7" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="X7" s="4" t="str" cm="1">
+        <f t="array" ref="X7">INDEX({"Satisfactory","Impressive","Outstanding"},MAX(1,ROUND(AVERAGE(MATCH(O7:R7,{"Satisfactory","Impressive","Outstanding"},0)),0)))</f>
+        <v>Impressive</v>
+      </c>
+      <c r="Y7" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z7" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="4">
+        <v>7</v>
+      </c>
+      <c r="B8" s="6">
+        <v>45770</v>
+      </c>
+      <c r="C8" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="4">
+        <v>1</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="L8" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="M8" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="N8" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="O8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="P8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="R8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="S8" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="T8" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="U8" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="V8" s="4">
+        <v>5</v>
+      </c>
+      <c r="W8" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="X8" s="4" t="str" cm="1">
+        <f t="array" ref="X8">INDEX({"Satisfactory","Impressive","Outstanding"},MAX(1,ROUND(AVERAGE(MATCH(O8:R8,{"Satisfactory","Impressive","Outstanding"},0)),0)))</f>
+        <v>Impressive</v>
+      </c>
+      <c r="Y8" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z8" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="4">
+        <v>8</v>
+      </c>
+      <c r="B9" s="6">
+        <v>45770</v>
+      </c>
+      <c r="C9" s="7">
+        <v>7.7777777777777779E-2</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="4">
+        <v>4</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="K9" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="L9" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="M9" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="N9" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="O9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="P9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="R9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="S9" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="T9" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="U9" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="V9" s="4">
+        <v>6</v>
+      </c>
+      <c r="W9" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="X9" s="4" t="str" cm="1">
+        <f t="array" ref="X9">INDEX({"Satisfactory","Impressive","Outstanding"},MAX(1,ROUND(AVERAGE(MATCH(O9:R9,{"Satisfactory","Impressive","Outstanding"},0)),0)))</f>
+        <v>Impressive</v>
+      </c>
+      <c r="Y9" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z9" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="Z1" s="8" t="s">
+    </row>
+    <row r="10" spans="1:34" ht="29" x14ac:dyDescent="0.35">
+      <c r="A10" s="4">
+        <v>9</v>
+      </c>
+      <c r="B10" s="6">
+        <v>45770</v>
+      </c>
+      <c r="C10" s="7">
+        <v>6.805555555555555E-2</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="4">
+        <v>4</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="I10" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="J10" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="K10" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="L10" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="M10" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="N10" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="O10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="P10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="R10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="S10" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="T10" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="U10" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="V10" s="4">
+        <v>7</v>
+      </c>
+      <c r="W10" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="X10" s="4" t="str" cm="1">
+        <f t="array" ref="X10">INDEX({"Satisfactory","Impressive","Outstanding"},MAX(1,ROUND(AVERAGE(MATCH(O10:R10,{"Satisfactory","Impressive","Outstanding"},0)),0)))</f>
+        <v>Impressive</v>
+      </c>
+      <c r="Y10" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z10" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="4">
+        <v>10</v>
+      </c>
+      <c r="B11" s="6">
+        <v>45770</v>
+      </c>
+      <c r="C11" s="7">
+        <v>0.48749999999999999</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="4">
+        <v>4</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="J11" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="K11" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="L11" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="M11" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="N11" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="O11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="P11" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="AA1" s="9">
-        <v>3</v>
+      <c r="Q11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="R11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="S11" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="T11" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="U11" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="V11" s="4">
+        <v>8</v>
+      </c>
+      <c r="W11" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="X11" s="4" t="str" cm="1">
+        <f t="array" ref="X11">INDEX({"Satisfactory","Impressive","Outstanding"},MAX(1,ROUND(AVERAGE(MATCH(O11:R11,{"Satisfactory","Impressive","Outstanding"},0)),0)))</f>
+        <v>Impressive</v>
+      </c>
+      <c r="Y11" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z11" s="4" t="s">
+        <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1" t="e" cm="1">
-        <f t="array" ref="N2">INDEX({"Satisfactory","Impressive","Outstanding"},MAX(1,ROUND(AVERAGE(MATCH(I2:M2,{"Satisfactory","Impressive","Outstanding"},0)),0)))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
-      <c r="Z2" s="8" t="s">
+    <row r="12" spans="1:34" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="4">
+        <v>11</v>
+      </c>
+      <c r="B12" s="6">
+        <v>45770</v>
+      </c>
+      <c r="C12" s="7">
+        <v>4.1666666666666666E-3</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="4">
+        <v>4</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="H12" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="I12" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="J12" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="K12" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="L12" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="M12" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="N12" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="O12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="P12" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="AA2" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A3" s="2"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1" t="e" cm="1">
-        <f t="array" ref="N3">INDEX({"Satisfactory","Impressive","Outstanding"},MAX(1,ROUND(AVERAGE(MATCH(I3:M3,{"Satisfactory","Impressive","Outstanding"},0)),0)))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="1"/>
-      <c r="S3" s="1"/>
-      <c r="Z3" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="AA3" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A4" s="2"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1" t="e" cm="1">
-        <f t="array" ref="N4">INDEX({"Satisfactory","Impressive","Outstanding"},MAX(1,ROUND(AVERAGE(MATCH(I4:M4,{"Satisfactory","Impressive","Outstanding"},0)),0)))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="1"/>
-      <c r="S4" s="1"/>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A5" s="2"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1" t="e" cm="1">
-        <f t="array" ref="N5">INDEX({"Satisfactory","Impressive","Outstanding"},MAX(1,ROUND(AVERAGE(MATCH(I5:M5,{"Satisfactory","Impressive","Outstanding"},0)),0)))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="1"/>
-      <c r="R5" s="1"/>
-      <c r="S5" s="1"/>
+      <c r="Q12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="R12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="S12" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="T12" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="U12" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="V12" s="4">
+        <v>9</v>
+      </c>
+      <c r="W12" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="X12" s="4" t="str" cm="1">
+        <f t="array" ref="X12">INDEX({"Satisfactory","Impressive","Outstanding"},MAX(1,ROUND(AVERAGE(MATCH(O12:R12,{"Satisfactory","Impressive","Outstanding"},0)),0)))</f>
+        <v>Impressive</v>
+      </c>
+      <c r="Y12" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z12" s="4" t="s">
+        <v>21</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="19" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="I3" r:id="rId1" display="vikas.datika@sgvgroup.in;neeraj.balodi@sgvgroup.in" xr:uid="{F5409571-8928-4BE1-AB8F-0CC5606A0600}"/>
+    <hyperlink ref="H4" r:id="rId2" xr:uid="{0E304B86-2DC2-439A-BE1F-366D2DE89209}"/>
+    <hyperlink ref="H3" r:id="rId3" xr:uid="{38AFF209-8BEF-40AA-B424-BF1A27CA6775}"/>
+    <hyperlink ref="H11:H12" r:id="rId4" display="rajesh.dahiya@sgvgroup.in" xr:uid="{EAFA755E-EDCD-40C5-8614-F86962E22F51}"/>
+    <hyperlink ref="H10" r:id="rId5" xr:uid="{B119FD6D-F8F9-4550-893F-679982907939}"/>
+    <hyperlink ref="H9" r:id="rId6" xr:uid="{564ADBAC-634F-450A-A9BF-71D86556091C}"/>
+    <hyperlink ref="I3:I12" r:id="rId7" display="vikas.datika@sgvgroup.in" xr:uid="{D5F975FB-8FFF-4975-8B4C-1205865E9414}"/>
+    <hyperlink ref="I2" r:id="rId8" display="vikas.datika@sgvgroup.in,neeraj.balodi@sgvgroup.in" xr:uid="{08DC5917-FF63-4E8B-927B-C7FEF20980E4}"/>
+    <hyperlink ref="H2" r:id="rId9" xr:uid="{CE5BCF97-E672-40A9-AFE1-89223E63FDDE}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>